<commit_message>
general and dbms tests fixes
</commit_message>
<xml_diff>
--- a/Developement/ITPD/Test_ste.xlsx
+++ b/Developement/ITPD/Test_ste.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>test case identifier</t>
   </si>
@@ -43,24 +43,12 @@
     <t>Check if Data Access Manager is able to communicate with and query the DBMS</t>
   </si>
   <si>
-    <t>Check if Query result is correct</t>
+    <t>Correct generation of the answer by the DBMS</t>
   </si>
   <si>
     <t>none</t>
   </si>
   <si>
-    <t>DBMS_I2T1</t>
-  </si>
-  <si>
-    <t>Request to the Data Access Manager for a specific Query to the DBMS</t>
-  </si>
-  <si>
-    <t>Check if the Data Access Manager is able to translate a request into the right query</t>
-  </si>
-  <si>
-    <t>DBMS_I1T1 succeeded, simple Application Controller Driver</t>
-  </si>
-  <si>
     <t>G_I1T1</t>
   </si>
   <si>
@@ -70,13 +58,13 @@
     <t>Request from a righteous client to do an action</t>
   </si>
   <si>
-    <t xml:space="preserve">Check if the Security Manager can check if a client has the right to do an action </t>
-  </si>
-  <si>
-    <t>Confirmation from the Security Manager that the client is able to do the action</t>
-  </si>
-  <si>
-    <t>Communication Subsystem Tests succeeded</t>
+    <t>Check if the Security Manager is able to forward actions from clients that have the rights to do them</t>
+  </si>
+  <si>
+    <t>Security Manager calls the right methods necessary to forward the action</t>
+  </si>
+  <si>
+    <t>Communication Subsystem and Security Manager Tests succeeded</t>
   </si>
   <si>
     <t>G_I1T2</t>
@@ -85,7 +73,10 @@
     <t>Request from a non-righteous client to do an action</t>
   </si>
   <si>
-    <t>Denial from the Security Manager</t>
+    <t>Check if the Security Manager can block actions from clients that don't have the rights to do them</t>
+  </si>
+  <si>
+    <t>Security Manager calls the right methods necessary to block the action and alert the client</t>
   </si>
   <si>
     <t>G_I2T1</t>
@@ -97,13 +88,13 @@
     <t xml:space="preserve">Request from the Security Manager for a tuple in the DBMS </t>
   </si>
   <si>
-    <t>Check if the Data Subsystem can answer the Security Manager</t>
-  </si>
-  <si>
-    <t>Check if the Tuple returned is the right one</t>
-  </si>
-  <si>
-    <t>Data Subsystem Tests Succeeded</t>
+    <t>Check if the Data Subsystem can receive Security Manager requests for data</t>
+  </si>
+  <si>
+    <t>Check if the DBMS chooses the right tuple</t>
+  </si>
+  <si>
+    <t>Data Subsystem and Security Manager Tests Succeeded</t>
   </si>
   <si>
     <t>G_I3T1</t>
@@ -115,13 +106,13 @@
     <t xml:space="preserve">Request from the Security Manager to do an action </t>
   </si>
   <si>
-    <t>Check if the Application Subsystem is able to execute an action requested by the Security Manager</t>
-  </si>
-  <si>
-    <t>Action confirmed</t>
-  </si>
-  <si>
-    <t>Application Subsystem Tests Succeeded</t>
+    <t>Check if the Application Subsystem is able to execute the right action requested by the Security Manager</t>
+  </si>
+  <si>
+    <t>The Application subsystem called the methods needed</t>
+  </si>
+  <si>
+    <t>Application Subsystem and Security Manager Tests Succeeded</t>
   </si>
   <si>
     <t>G_I4T1</t>
@@ -133,13 +124,31 @@
     <t xml:space="preserve">Request from the Application Subsystem for data </t>
   </si>
   <si>
-    <t>Check if the Data Subsystem can answer correctly requests from the Application Subsystem</t>
-  </si>
-  <si>
-    <t>Data returned correctly</t>
+    <t>Check if the Data Subsystem can generate the correct queries after being questioned by the Application Subsystem</t>
+  </si>
+  <si>
+    <t>The Data Subsystem called the right methods</t>
   </si>
   <si>
     <t>Application Subsystem Tests and Data Subsystem Tests Succeeded</t>
+  </si>
+  <si>
+    <t>G_I5T1</t>
+  </si>
+  <si>
+    <t>Application Subsystem -&gt; Communication Subsystem</t>
+  </si>
+  <si>
+    <t>Notification from the Application subsystem directed to a client</t>
+  </si>
+  <si>
+    <t>Check if the Communication Subsystem receives the right informations from the Application Subsystem</t>
+  </si>
+  <si>
+    <t>Notification received correctly</t>
+  </si>
+  <si>
+    <t>Application Subsystem and Communication Subsystem tests succeeded</t>
   </si>
 </sst>
 </file>
@@ -200,7 +209,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="16.29"/>
-    <col customWidth="1" min="3" max="3" width="18.86"/>
+    <col customWidth="1" min="3" max="3" width="41.29"/>
     <col customWidth="1" min="4" max="4" width="16.43"/>
     <col customWidth="1" min="6" max="6" width="17.86"/>
     <col customWidth="1" min="7" max="7" width="18.29"/>
@@ -247,123 +256,130 @@
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="G4" s="1"/>
     </row>
     <row r="6">
       <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="1" t="s">
+    </row>
+    <row r="11">
+      <c r="B11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>42</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>